<commit_message>
moving pieces around and generating more card types
</commit_message>
<xml_diff>
--- a/game-files/cards.xlsx
+++ b/game-files/cards.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="95">
   <si>
     <t>capacity</t>
   </si>
@@ -295,6 +295,12 @@
   </si>
   <si>
     <t>effect</t>
+  </si>
+  <si>
+    <t>Can play "+" cards as "-" cards</t>
+  </si>
+  <si>
+    <t>Political chaos</t>
   </si>
 </sst>
 </file>
@@ -644,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S42"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O42" sqref="O42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2682,10 +2688,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2891,6 +2897,20 @@
         <v>89</v>
       </c>
     </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>93</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
addressing issues after first tests
</commit_message>
<xml_diff>
--- a/game-files/cards.xlsx
+++ b/game-files/cards.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Cards" sheetId="1" r:id="rId1"/>
@@ -75,9 +75,6 @@
     <t>Gather support from foreign diplomats</t>
   </si>
   <si>
-    <t>Negative statement from Ministry of Economy</t>
-  </si>
-  <si>
     <t>Playable in segment</t>
   </si>
   <si>
@@ -301,6 +298,9 @@
   </si>
   <si>
     <t>Political chaos</t>
+  </si>
+  <si>
+    <t>Lobby foreign diplomats to damage proposal</t>
   </si>
 </sst>
 </file>
@@ -650,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O42" sqref="O42"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -664,13 +664,13 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -691,7 +691,7 @@
         <v>5</v>
       </c>
       <c r="J1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L1" t="s">
         <v>7</v>
@@ -703,19 +703,19 @@
         <v>8</v>
       </c>
       <c r="O1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P1" t="s">
         <v>58</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>59</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>60</v>
       </c>
-      <c r="R1" t="s">
-        <v>61</v>
-      </c>
       <c r="S1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
@@ -779,7 +779,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>94</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -788,7 +788,7 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="F3">
         <v>-1</v>
@@ -804,7 +804,7 @@
       </c>
       <c r="J3">
         <f t="shared" ref="J3:J33" si="0">SUM(D3:I3)</f>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="M3">
         <v>-1</v>
@@ -834,7 +834,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -886,7 +886,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5">
         <v>-1</v>
@@ -917,7 +917,7 @@
         <v>0</v>
       </c>
       <c r="O5">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="P5">
         <v>-1</v>
@@ -930,7 +930,7 @@
       </c>
       <c r="S5">
         <f t="shared" si="1"/>
-        <v>-2</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
@@ -993,7 +993,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1097,7 +1097,7 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9">
         <v>-1</v>
@@ -1106,7 +1106,7 @@
         <v>-1</v>
       </c>
       <c r="F9">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -1119,7 +1119,7 @@
       </c>
       <c r="J9">
         <f t="shared" si="0"/>
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="M9">
         <v>0</v>
@@ -1149,7 +1149,7 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1186,14 +1186,14 @@
         <v>0</v>
       </c>
       <c r="Q10">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="R10">
         <v>0</v>
       </c>
       <c r="S10">
         <f t="shared" si="1"/>
-        <v>-1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
@@ -1253,7 +1253,7 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -1305,7 +1305,7 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1360,7 +1360,7 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -1415,7 +1415,7 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -1486,11 +1486,11 @@
       </c>
       <c r="E17" s="1">
         <f t="shared" ref="E17:J17" si="2">SUMPRODUCT($A2:$A16, E2:E16)</f>
-        <v>-31</v>
+        <v>-33</v>
       </c>
       <c r="F17" s="1">
         <f t="shared" si="2"/>
-        <v>-26</v>
+        <v>-23</v>
       </c>
       <c r="G17" s="1">
         <f t="shared" si="2"/>
@@ -1506,7 +1506,7 @@
       </c>
       <c r="J17" s="1">
         <f t="shared" si="2"/>
-        <v>-113</v>
+        <v>-112</v>
       </c>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -1520,7 +1520,7 @@
       </c>
       <c r="O17" s="1">
         <f t="shared" ref="O17" si="5">SUMPRODUCT($A2:$A16, O2:O16)</f>
-        <v>-15</v>
+        <v>-18</v>
       </c>
       <c r="P17" s="1">
         <f t="shared" ref="P17" si="6">SUMPRODUCT($A2:$A16, P2:P16)</f>
@@ -1528,7 +1528,7 @@
       </c>
       <c r="Q17" s="1">
         <f t="shared" ref="Q17" si="7">SUMPRODUCT($A2:$A16, Q2:Q16)</f>
-        <v>-15</v>
+        <v>-18</v>
       </c>
       <c r="R17" s="1">
         <f t="shared" ref="R17" si="8">SUMPRODUCT($A2:$A16, R2:R16)</f>
@@ -1536,7 +1536,7 @@
       </c>
       <c r="S17" s="1">
         <f t="shared" ref="S17" si="9">SUMPRODUCT($A2:$A16, S2:S16)</f>
-        <v>-78</v>
+        <v>-84</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
@@ -1546,11 +1546,11 @@
       </c>
       <c r="E18" s="1">
         <f t="shared" ref="E18:R18" si="10">AVERAGE(E2:E16)</f>
-        <v>-0.8571428571428571</v>
+        <v>-0.9285714285714286</v>
       </c>
       <c r="F18" s="1">
         <f t="shared" si="10"/>
-        <v>-0.7142857142857143</v>
+        <v>-0.6428571428571429</v>
       </c>
       <c r="G18" s="1">
         <f t="shared" si="10"/>
@@ -1580,7 +1580,7 @@
       </c>
       <c r="O18" s="1">
         <f t="shared" si="10"/>
-        <v>-0.42857142857142855</v>
+        <v>-0.5</v>
       </c>
       <c r="P18" s="1">
         <f t="shared" si="10"/>
@@ -1588,7 +1588,7 @@
       </c>
       <c r="Q18" s="1">
         <f t="shared" si="10"/>
-        <v>-0.35714285714285715</v>
+        <v>-0.42857142857142855</v>
       </c>
       <c r="R18" s="1">
         <f t="shared" si="10"/>
@@ -1596,7 +1596,7 @@
       </c>
       <c r="S18">
         <f t="shared" si="1"/>
-        <v>-2.1428571428571428</v>
+        <v>-2.2857142857142856</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
@@ -1714,7 +1714,7 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -1766,7 +1766,7 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -2026,7 +2026,7 @@
         <v>2</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C28">
         <v>2</v>
@@ -2081,7 +2081,7 @@
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -2133,7 +2133,7 @@
         <v>2</v>
       </c>
       <c r="B30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C30">
         <v>2</v>
@@ -2188,7 +2188,7 @@
         <v>2</v>
       </c>
       <c r="B31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C31">
         <v>2</v>
@@ -2243,7 +2243,7 @@
         <v>3</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D32">
         <v>-2</v>
@@ -2283,11 +2283,11 @@
         <v>0</v>
       </c>
       <c r="R32">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S32">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.3">
@@ -2357,11 +2357,11 @@
       </c>
       <c r="R34" s="1">
         <f t="shared" ref="R34" si="17">SUMPRODUCT($A20:$A33,R20:R33)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="S34" s="1">
         <f t="shared" ref="S34" si="18">SUMPRODUCT($A20:$A33,S20:S33)</f>
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.3">
@@ -2417,11 +2417,11 @@
       </c>
       <c r="R35" s="1">
         <f t="shared" si="19"/>
-        <v>0.15384615384615385</v>
+        <v>0.23076923076923078</v>
       </c>
       <c r="S35">
         <f t="shared" si="1"/>
-        <v>2.2307692307692304</v>
+        <v>2.3076923076923075</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.3">
@@ -2435,7 +2435,7 @@
         <v>5</v>
       </c>
       <c r="B37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D37">
         <v>-1</v>
@@ -2500,11 +2500,11 @@
       </c>
       <c r="E42">
         <f t="shared" si="20"/>
-        <v>-48</v>
+        <v>-50</v>
       </c>
       <c r="F42">
         <f t="shared" si="20"/>
-        <v>-44</v>
+        <v>-41</v>
       </c>
       <c r="G42">
         <f t="shared" si="20"/>
@@ -2520,7 +2520,7 @@
       </c>
       <c r="J42">
         <f t="shared" si="20"/>
-        <v>-219</v>
+        <v>-218</v>
       </c>
       <c r="M42">
         <f t="shared" ref="M42:R42" si="21">M17+M34</f>
@@ -2532,7 +2532,7 @@
       </c>
       <c r="O42">
         <f t="shared" si="21"/>
-        <v>-1</v>
+        <v>-4</v>
       </c>
       <c r="P42">
         <f t="shared" si="21"/>
@@ -2540,11 +2540,11 @@
       </c>
       <c r="Q42">
         <f t="shared" si="21"/>
-        <v>-6</v>
+        <v>-9</v>
       </c>
       <c r="R42">
         <f t="shared" si="21"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -2568,77 +2568,77 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B26">
         <v>22</v>
@@ -2646,7 +2646,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B27">
         <v>10</v>
@@ -2654,7 +2654,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B28">
         <f>B27/4</f>
@@ -2669,7 +2669,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B31">
         <v>2</v>
@@ -2690,8 +2690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2703,212 +2703,212 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
         <v>91</v>
-      </c>
-      <c r="B1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
         <v>80</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
         <v>88</v>
-      </c>
-      <c r="B14">
-        <v>3</v>
-      </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="D14" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B15">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>